<commit_message>
Big belated code dump including but not limited to new figures, curations, and a new alternative draft model
</commit_message>
<xml_diff>
--- a/data/clean/CUE2/cue2.xlsx
+++ b/data/clean/CUE2/cue2.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27628"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28227"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/a30fe02b4181869d/SchoolWork/Stanford Grad/Projects/Covert Lab/Oceans/rpom-fba/data/clean/CUE2/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="379" documentId="8_{E1D00C96-A94C-41A2-8D46-00455408C892}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{F51F2D64-0355-4079-AD8D-1D5FD5226247}"/>
+  <xr:revisionPtr revIDLastSave="380" documentId="8_{E1D00C96-A94C-41A2-8D46-00455408C892}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{5436C360-50B2-42B1-B59F-5FF488EB1B6E}"/>
   <bookViews>
-    <workbookView minimized="1" xWindow="45" yWindow="180" windowWidth="24360" windowHeight="22875" activeTab="1" xr2:uid="{C524C702-4B68-407C-8914-DBC658242935}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="15500" activeTab="5" xr2:uid="{C524C702-4B68-407C-8914-DBC658242935}"/>
   </bookViews>
   <sheets>
     <sheet name="Cell number" sheetId="1" r:id="rId1"/>
@@ -42,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="128" uniqueCount="57">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="127" uniqueCount="56">
   <si>
     <t>Calculated cell number  (Cells ml-1)</t>
   </si>
@@ -155,9 +155,6 @@
     <t>8gluc_4ace_F</t>
   </si>
   <si>
-    <t xml:space="preserve"> </t>
-  </si>
-  <si>
     <t>Glucose_mean</t>
   </si>
   <si>
@@ -223,7 +220,7 @@
     <numFmt numFmtId="164" formatCode="0.0000"/>
     <numFmt numFmtId="165" formatCode="0.000"/>
     <numFmt numFmtId="166" formatCode="0.0"/>
-    <numFmt numFmtId="170" formatCode="0.000000"/>
+    <numFmt numFmtId="167" formatCode="0.000000"/>
   </numFmts>
   <fonts count="3" x14ac:knownFonts="1">
     <font>
@@ -294,7 +291,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="20">
+  <cellXfs count="19">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="11" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -314,9 +311,8 @@
     <xf numFmtId="11" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="164" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="170" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -2102,22 +2098,22 @@
       <selection activeCell="AC3" sqref="AC3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="7" width="12.42578125" style="2"/>
-    <col min="8" max="8" width="18.85546875" style="2" bestFit="1" customWidth="1"/>
-    <col min="9" max="14" width="12.42578125" style="2"/>
-    <col min="15" max="15" width="18.5703125" style="2" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="13.5703125" bestFit="1" customWidth="1"/>
+    <col min="1" max="7" width="12.453125" style="2"/>
+    <col min="8" max="8" width="18.81640625" style="2" bestFit="1" customWidth="1"/>
+    <col min="9" max="14" width="12.453125" style="2"/>
+    <col min="15" max="15" width="18.54296875" style="2" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="13.54296875" bestFit="1" customWidth="1"/>
     <col min="17" max="17" width="14" bestFit="1" customWidth="1"/>
-    <col min="18" max="21" width="12.42578125" style="2"/>
-    <col min="22" max="22" width="21.7109375" style="2" customWidth="1"/>
-    <col min="23" max="28" width="12.42578125" style="2"/>
-    <col min="29" max="29" width="21.7109375" style="2" bestFit="1" customWidth="1"/>
-    <col min="30" max="30" width="12.42578125" style="2"/>
+    <col min="18" max="21" width="12.453125" style="2"/>
+    <col min="22" max="22" width="21.7265625" style="2" customWidth="1"/>
+    <col min="23" max="28" width="12.453125" style="2"/>
+    <col min="29" max="29" width="21.7265625" style="2" bestFit="1" customWidth="1"/>
+    <col min="30" max="30" width="12.453125" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:30" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:30" ht="16" x14ac:dyDescent="0.4">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -2150,7 +2146,7 @@
       <c r="AC1" s="1"/>
       <c r="AD1" s="1"/>
     </row>
-    <row r="2" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:30" x14ac:dyDescent="0.35">
       <c r="A2" s="2" t="s">
         <v>1</v>
       </c>
@@ -2173,7 +2169,7 @@
         <v>7</v>
       </c>
       <c r="H2" s="14" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="I2" s="2" t="s">
         <v>8</v>
@@ -2194,52 +2190,52 @@
         <v>13</v>
       </c>
       <c r="O2" s="14" t="s">
+        <v>38</v>
+      </c>
+      <c r="P2" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="Q2" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="R2" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="S2" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="T2" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="U2" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="V2" s="14" t="s">
         <v>39</v>
       </c>
-      <c r="P2" s="2" t="s">
-        <v>48</v>
-      </c>
-      <c r="Q2" s="2" t="s">
-        <v>49</v>
-      </c>
-      <c r="R2" s="2" t="s">
-        <v>50</v>
-      </c>
-      <c r="S2" s="2" t="s">
-        <v>51</v>
-      </c>
-      <c r="T2" s="2" t="s">
-        <v>52</v>
-      </c>
-      <c r="U2" s="2" t="s">
+      <c r="W2" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="X2" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="Y2" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="Z2" s="2" t="s">
         <v>53</v>
       </c>
-      <c r="V2" s="14" t="s">
+      <c r="AA2" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="AB2" s="2" t="s">
+        <v>55</v>
+      </c>
+      <c r="AC2" s="14" t="s">
         <v>40</v>
       </c>
-      <c r="W2" s="2" t="s">
-        <v>45</v>
-      </c>
-      <c r="X2" s="2" t="s">
-        <v>47</v>
-      </c>
-      <c r="Y2" s="2" t="s">
-        <v>46</v>
-      </c>
-      <c r="Z2" s="2" t="s">
-        <v>54</v>
-      </c>
-      <c r="AA2" s="2" t="s">
-        <v>55</v>
-      </c>
-      <c r="AB2" s="2" t="s">
-        <v>56</v>
-      </c>
-      <c r="AC2" s="14" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="3" spans="1:30" x14ac:dyDescent="0.25">
+    </row>
+    <row r="3" spans="1:30" x14ac:dyDescent="0.35">
       <c r="A3" s="10">
         <v>0.5</v>
       </c>
@@ -2332,7 +2328,7 @@
         <v>2874999.9999999814</v>
       </c>
     </row>
-    <row r="4" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:30" x14ac:dyDescent="0.35">
       <c r="A4" s="10">
         <v>1</v>
       </c>
@@ -2355,7 +2351,7 @@
         <v>0</v>
       </c>
       <c r="H4" s="2">
-        <f t="shared" ref="H4:H58" si="0">AVERAGE(B4:G4)</f>
+        <f t="shared" ref="H4:H57" si="0">AVERAGE(B4:G4)</f>
         <v>4333333.3333333554</v>
       </c>
       <c r="I4" s="2">
@@ -2425,7 +2421,7 @@
         <v>2249999.9999999884</v>
       </c>
     </row>
-    <row r="5" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:30" x14ac:dyDescent="0.35">
       <c r="A5" s="10">
         <v>1.5</v>
       </c>
@@ -2514,11 +2510,11 @@
         <v>0</v>
       </c>
       <c r="AC5" s="2">
-        <f t="shared" ref="AC4:AC58" si="3">AVERAGE(W5:AB5)</f>
+        <f t="shared" ref="AC5:AC58" si="3">AVERAGE(W5:AB5)</f>
         <v>124999.99999999318</v>
       </c>
     </row>
-    <row r="6" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:30" x14ac:dyDescent="0.35">
       <c r="A6" s="10">
         <v>2</v>
       </c>
@@ -2611,7 +2607,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:30" x14ac:dyDescent="0.35">
       <c r="A7" s="10">
         <v>2.5</v>
       </c>
@@ -2704,7 +2700,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:30" x14ac:dyDescent="0.35">
       <c r="A8" s="10">
         <v>3</v>
       </c>
@@ -2797,7 +2793,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:30" x14ac:dyDescent="0.35">
       <c r="A9" s="10">
         <v>3.5</v>
       </c>
@@ -2890,7 +2886,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:30" x14ac:dyDescent="0.35">
       <c r="A10" s="10">
         <v>4</v>
       </c>
@@ -2983,7 +2979,7 @@
         <v>124999.99999999318</v>
       </c>
     </row>
-    <row r="11" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:30" x14ac:dyDescent="0.35">
       <c r="A11" s="10">
         <v>4.5</v>
       </c>
@@ -3076,7 +3072,7 @@
         <v>624999.9999999936</v>
       </c>
     </row>
-    <row r="12" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:30" x14ac:dyDescent="0.35">
       <c r="A12" s="10">
         <v>5</v>
       </c>
@@ -3169,7 +3165,7 @@
         <v>10749999.999999989</v>
       </c>
     </row>
-    <row r="13" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:30" x14ac:dyDescent="0.35">
       <c r="A13" s="10">
         <v>5.5</v>
       </c>
@@ -3262,7 +3258,7 @@
         <v>37499999.999999978</v>
       </c>
     </row>
-    <row r="14" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:30" x14ac:dyDescent="0.35">
       <c r="A14" s="10">
         <v>6</v>
       </c>
@@ -3355,7 +3351,7 @@
         <v>42499999.999999978</v>
       </c>
     </row>
-    <row r="15" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:30" x14ac:dyDescent="0.35">
       <c r="A15" s="10">
         <v>6.5</v>
       </c>
@@ -3448,7 +3444,7 @@
         <v>39499999.999999985</v>
       </c>
     </row>
-    <row r="16" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:30" x14ac:dyDescent="0.35">
       <c r="A16" s="10">
         <v>7</v>
       </c>
@@ -3541,7 +3537,7 @@
         <v>43249999.999999978</v>
       </c>
     </row>
-    <row r="17" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:29" x14ac:dyDescent="0.35">
       <c r="A17" s="10">
         <v>7.5</v>
       </c>
@@ -3634,7 +3630,7 @@
         <v>42624999.999999978</v>
       </c>
     </row>
-    <row r="18" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:29" x14ac:dyDescent="0.35">
       <c r="A18" s="10">
         <v>8</v>
       </c>
@@ -3727,7 +3723,7 @@
         <v>62250000</v>
       </c>
     </row>
-    <row r="19" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:29" x14ac:dyDescent="0.35">
       <c r="A19" s="10">
         <v>8.5</v>
       </c>
@@ -3820,7 +3816,7 @@
         <v>84749999.999999955</v>
       </c>
     </row>
-    <row r="20" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:29" x14ac:dyDescent="0.35">
       <c r="A20" s="10">
         <v>9</v>
       </c>
@@ -3913,7 +3909,7 @@
         <v>111749999.99999996</v>
       </c>
     </row>
-    <row r="21" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:29" x14ac:dyDescent="0.35">
       <c r="A21" s="10">
         <v>9.5</v>
       </c>
@@ -4006,7 +4002,7 @@
         <v>138749999.99999997</v>
       </c>
     </row>
-    <row r="22" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:29" x14ac:dyDescent="0.35">
       <c r="A22" s="10">
         <v>10</v>
       </c>
@@ -4099,7 +4095,7 @@
         <v>167250000</v>
       </c>
     </row>
-    <row r="23" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:29" x14ac:dyDescent="0.35">
       <c r="A23" s="10">
         <v>10.5</v>
       </c>
@@ -4192,7 +4188,7 @@
         <v>197749999.99999997</v>
       </c>
     </row>
-    <row r="24" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:29" x14ac:dyDescent="0.35">
       <c r="A24" s="10">
         <v>11</v>
       </c>
@@ -4285,7 +4281,7 @@
         <v>219249999.99999997</v>
       </c>
     </row>
-    <row r="25" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:29" x14ac:dyDescent="0.35">
       <c r="A25" s="10">
         <v>11.5</v>
       </c>
@@ -4378,7 +4374,7 @@
         <v>230249999.99999997</v>
       </c>
     </row>
-    <row r="26" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:29" x14ac:dyDescent="0.35">
       <c r="A26" s="10">
         <v>12</v>
       </c>
@@ -4471,7 +4467,7 @@
         <v>236749999.99999997</v>
       </c>
     </row>
-    <row r="27" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:29" x14ac:dyDescent="0.35">
       <c r="A27" s="10">
         <v>12.5</v>
       </c>
@@ -4564,7 +4560,7 @@
         <v>244750000</v>
       </c>
     </row>
-    <row r="28" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:29" x14ac:dyDescent="0.35">
       <c r="A28" s="10">
         <v>13</v>
       </c>
@@ -4657,7 +4653,7 @@
         <v>255750000</v>
       </c>
     </row>
-    <row r="29" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:29" x14ac:dyDescent="0.35">
       <c r="A29" s="10">
         <v>13.5</v>
       </c>
@@ -4750,7 +4746,7 @@
         <v>272750000</v>
       </c>
     </row>
-    <row r="30" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:29" x14ac:dyDescent="0.35">
       <c r="A30" s="10">
         <v>14</v>
       </c>
@@ -4843,7 +4839,7 @@
         <v>292749999.99999994</v>
       </c>
     </row>
-    <row r="31" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:29" x14ac:dyDescent="0.35">
       <c r="A31" s="10">
         <v>14.5</v>
       </c>
@@ -4936,7 +4932,7 @@
         <v>320250000</v>
       </c>
     </row>
-    <row r="32" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:29" x14ac:dyDescent="0.35">
       <c r="A32" s="10">
         <v>15</v>
       </c>
@@ -5029,7 +5025,7 @@
         <v>350250000</v>
       </c>
     </row>
-    <row r="33" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:29" x14ac:dyDescent="0.35">
       <c r="A33" s="10">
         <v>15.5</v>
       </c>
@@ -5122,7 +5118,7 @@
         <v>383249999.99999994</v>
       </c>
     </row>
-    <row r="34" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:29" x14ac:dyDescent="0.35">
       <c r="A34" s="10">
         <v>16</v>
       </c>
@@ -5215,7 +5211,7 @@
         <v>422250000</v>
       </c>
     </row>
-    <row r="35" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:29" x14ac:dyDescent="0.35">
       <c r="A35" s="10">
         <v>16.5</v>
       </c>
@@ -5308,7 +5304,7 @@
         <v>463750000</v>
       </c>
     </row>
-    <row r="36" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:29" x14ac:dyDescent="0.35">
       <c r="A36" s="10">
         <v>17</v>
       </c>
@@ -5401,7 +5397,7 @@
         <v>510249999.99999994</v>
       </c>
     </row>
-    <row r="37" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:29" x14ac:dyDescent="0.35">
       <c r="A37" s="10">
         <v>17.5</v>
       </c>
@@ -5494,7 +5490,7 @@
         <v>557250000</v>
       </c>
     </row>
-    <row r="38" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:29" x14ac:dyDescent="0.35">
       <c r="A38" s="10">
         <v>18</v>
       </c>
@@ -5587,7 +5583,7 @@
         <v>588750000</v>
       </c>
     </row>
-    <row r="39" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:29" x14ac:dyDescent="0.35">
       <c r="A39" s="10">
         <v>18.5</v>
       </c>
@@ -5680,7 +5676,7 @@
         <v>590750000</v>
       </c>
     </row>
-    <row r="40" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:29" x14ac:dyDescent="0.35">
       <c r="A40" s="10">
         <v>19</v>
       </c>
@@ -5773,7 +5769,7 @@
         <v>585750000</v>
       </c>
     </row>
-    <row r="41" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:29" x14ac:dyDescent="0.35">
       <c r="A41" s="10">
         <v>19.5</v>
       </c>
@@ -5866,7 +5862,7 @@
         <v>579749999.99999988</v>
       </c>
     </row>
-    <row r="42" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:29" x14ac:dyDescent="0.35">
       <c r="A42" s="10">
         <v>20</v>
       </c>
@@ -5959,7 +5955,7 @@
         <v>573749999.99999988</v>
       </c>
     </row>
-    <row r="43" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:29" x14ac:dyDescent="0.35">
       <c r="A43" s="10">
         <v>20.5</v>
       </c>
@@ -6052,7 +6048,7 @@
         <v>571749999.99999988</v>
       </c>
     </row>
-    <row r="44" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:29" x14ac:dyDescent="0.35">
       <c r="A44" s="10">
         <v>21</v>
       </c>
@@ -6145,7 +6141,7 @@
         <v>568249999.99999988</v>
       </c>
     </row>
-    <row r="45" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:29" x14ac:dyDescent="0.35">
       <c r="A45" s="10">
         <v>21.5</v>
       </c>
@@ -6238,7 +6234,7 @@
         <v>564249999.99999988</v>
       </c>
     </row>
-    <row r="46" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:29" x14ac:dyDescent="0.35">
       <c r="A46" s="10">
         <v>22</v>
       </c>
@@ -6331,7 +6327,7 @@
         <v>560749999.99999988</v>
       </c>
     </row>
-    <row r="47" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:29" x14ac:dyDescent="0.35">
       <c r="A47" s="10">
         <v>22.5</v>
       </c>
@@ -6424,7 +6420,7 @@
         <v>558249999.99999988</v>
       </c>
     </row>
-    <row r="48" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:29" x14ac:dyDescent="0.35">
       <c r="A48" s="10">
         <v>23</v>
       </c>
@@ -6517,7 +6513,7 @@
         <v>556249999.99999988</v>
       </c>
     </row>
-    <row r="49" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:29" x14ac:dyDescent="0.35">
       <c r="A49" s="10">
         <v>23.5</v>
       </c>
@@ -6610,7 +6606,7 @@
         <v>557249999.99999988</v>
       </c>
     </row>
-    <row r="50" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:29" x14ac:dyDescent="0.35">
       <c r="A50" s="10">
         <v>24</v>
       </c>
@@ -6703,7 +6699,7 @@
         <v>553749999.99999988</v>
       </c>
     </row>
-    <row r="51" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:29" x14ac:dyDescent="0.35">
       <c r="A51" s="10">
         <v>24.5</v>
       </c>
@@ -6796,7 +6792,7 @@
         <v>552249999.99999988</v>
       </c>
     </row>
-    <row r="52" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:29" x14ac:dyDescent="0.35">
       <c r="A52" s="10">
         <v>25</v>
       </c>
@@ -6889,7 +6885,7 @@
         <v>553249999.99999988</v>
       </c>
     </row>
-    <row r="53" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:29" x14ac:dyDescent="0.35">
       <c r="A53" s="10">
         <v>25.5</v>
       </c>
@@ -6982,7 +6978,7 @@
         <v>548249999.99999988</v>
       </c>
     </row>
-    <row r="54" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:29" x14ac:dyDescent="0.35">
       <c r="A54" s="10">
         <v>26</v>
       </c>
@@ -7075,7 +7071,7 @@
         <v>545249999.99999988</v>
       </c>
     </row>
-    <row r="55" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:29" x14ac:dyDescent="0.35">
       <c r="A55" s="10">
         <v>26.5</v>
       </c>
@@ -7168,7 +7164,7 @@
         <v>542749999.99999988</v>
       </c>
     </row>
-    <row r="56" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:29" x14ac:dyDescent="0.35">
       <c r="A56" s="10">
         <v>27</v>
       </c>
@@ -7261,7 +7257,7 @@
         <v>542249999.99999988</v>
       </c>
     </row>
-    <row r="57" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:29" x14ac:dyDescent="0.35">
       <c r="A57" s="10">
         <v>27.5</v>
       </c>
@@ -7354,7 +7350,7 @@
         <v>542249999.99999988</v>
       </c>
     </row>
-    <row r="58" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:29" x14ac:dyDescent="0.35">
       <c r="A58" s="10">
         <v>28</v>
       </c>
@@ -7456,24 +7452,24 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B40DEBA3-5FEC-4BFC-9308-F58216F46179}">
   <dimension ref="A1:M18"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="O7" sqref="O7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="12.42578125" bestFit="1" customWidth="1"/>
-    <col min="5" max="6" width="13.42578125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="12.453125" bestFit="1" customWidth="1"/>
+    <col min="5" max="6" width="13.453125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A1" s="16" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.25">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="2" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B2" t="s">
         <v>2</v>
@@ -7485,28 +7481,28 @@
         <v>4</v>
       </c>
       <c r="E2" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="F2" t="s">
+        <v>47</v>
+      </c>
+      <c r="G2" t="s">
         <v>48</v>
       </c>
-      <c r="G2" t="s">
+      <c r="H2" t="s">
         <v>49</v>
       </c>
-      <c r="H2" t="s">
-        <v>50</v>
-      </c>
       <c r="I2" t="s">
+        <v>44</v>
+      </c>
+      <c r="J2" t="s">
+        <v>46</v>
+      </c>
+      <c r="K2" t="s">
         <v>45</v>
       </c>
-      <c r="J2" t="s">
-        <v>47</v>
-      </c>
-      <c r="K2" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
+    </row>
+    <row r="3" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A3">
         <v>0</v>
       </c>
@@ -7522,26 +7518,26 @@
       <c r="E3">
         <v>0</v>
       </c>
-      <c r="F3" s="19">
+      <c r="F3" s="18">
         <v>0.66666666666666674</v>
       </c>
-      <c r="G3" s="19">
+      <c r="G3" s="18">
         <v>0.66666666666666674</v>
       </c>
-      <c r="H3" s="19">
+      <c r="H3" s="18">
         <v>0.66666666666666674</v>
       </c>
-      <c r="I3" s="19">
+      <c r="I3" s="18">
         <v>1.3333333333333335</v>
       </c>
-      <c r="J3" s="19">
+      <c r="J3" s="18">
         <v>1.3333333333333335</v>
       </c>
-      <c r="K3" s="19">
+      <c r="K3" s="18">
         <v>1.3333333333333335</v>
       </c>
     </row>
-    <row r="4" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A4">
         <v>4.5</v>
       </c>
@@ -7557,26 +7553,26 @@
       <c r="E4">
         <v>4</v>
       </c>
-      <c r="F4" s="19">
+      <c r="F4" s="18">
         <v>0.66666666666666674</v>
       </c>
-      <c r="G4" s="19">
+      <c r="G4" s="18">
         <v>0.66666666666666674</v>
       </c>
-      <c r="H4" s="19">
+      <c r="H4" s="18">
         <v>0.65614421116666666</v>
       </c>
-      <c r="I4" s="19">
+      <c r="I4" s="18">
         <v>1.2641246318333332</v>
       </c>
-      <c r="J4" s="19">
+      <c r="J4" s="18">
         <v>1.3333333333333335</v>
       </c>
-      <c r="K4" s="19">
+      <c r="K4" s="18">
         <v>1.3333333333333335</v>
       </c>
     </row>
-    <row r="5" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A5">
         <v>8.5</v>
       </c>
@@ -7592,26 +7588,26 @@
       <c r="E5">
         <v>8</v>
       </c>
-      <c r="F5" s="19">
+      <c r="F5" s="18">
         <v>0.66666666666666674</v>
       </c>
-      <c r="G5" s="19">
+      <c r="G5" s="18">
         <v>0.66666666666666674</v>
       </c>
-      <c r="H5" s="19">
+      <c r="H5" s="18">
         <v>0.66666666666666674</v>
       </c>
-      <c r="I5" s="19">
+      <c r="I5" s="18">
         <v>1.2745792913333334</v>
       </c>
-      <c r="J5" s="19">
+      <c r="J5" s="18">
         <v>1.3333333333333335</v>
       </c>
-      <c r="K5" s="19">
+      <c r="K5" s="18">
         <v>1.3333333333333335</v>
       </c>
     </row>
-    <row r="6" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A6">
         <v>12.5</v>
       </c>
@@ -7627,26 +7623,26 @@
       <c r="E6">
         <v>12</v>
       </c>
-      <c r="F6" s="19">
+      <c r="F6" s="18">
         <v>0.60621889250000005</v>
       </c>
-      <c r="G6" s="19">
+      <c r="G6" s="18">
         <v>0.66666666666666674</v>
       </c>
-      <c r="H6" s="19">
+      <c r="H6" s="18">
         <v>0.61717897450000003</v>
       </c>
-      <c r="I6" s="19">
+      <c r="I6" s="18">
         <v>1.1909949536666666</v>
       </c>
-      <c r="J6" s="19">
+      <c r="J6" s="18">
         <v>1.2717160075</v>
       </c>
-      <c r="K6" s="19">
+      <c r="K6" s="18">
         <v>1.3333333333333335</v>
       </c>
     </row>
-    <row r="7" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A7">
         <v>15.5</v>
       </c>
@@ -7662,26 +7658,26 @@
       <c r="E7">
         <v>16.3</v>
       </c>
-      <c r="F7" s="19">
+      <c r="F7" s="18">
         <v>0.44645697883333335</v>
       </c>
-      <c r="G7" s="19">
+      <c r="G7" s="18">
         <v>0.44045816099999996</v>
       </c>
-      <c r="H7" s="19">
+      <c r="H7" s="18">
         <v>0.37168518433333331</v>
       </c>
-      <c r="I7" s="19">
+      <c r="I7" s="18">
         <v>0.79911268366666677</v>
       </c>
-      <c r="J7" s="19">
+      <c r="J7" s="18">
         <v>0.82344507933333333</v>
       </c>
-      <c r="K7" s="19">
+      <c r="K7" s="18">
         <v>1.0844775153333335</v>
       </c>
     </row>
-    <row r="8" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A8">
         <v>17.5</v>
       </c>
@@ -7697,26 +7693,26 @@
       <c r="E8">
         <v>20</v>
       </c>
-      <c r="F8" s="19">
+      <c r="F8" s="18">
         <v>0.20592278</v>
       </c>
-      <c r="G8" s="19">
+      <c r="G8" s="18">
         <v>0.11840804908333333</v>
       </c>
-      <c r="H8" s="19">
+      <c r="H8" s="18">
         <v>0.15753766459999999</v>
       </c>
-      <c r="I8" s="19">
+      <c r="I8" s="18">
         <v>0.30774034099999997</v>
       </c>
-      <c r="J8" s="19">
+      <c r="J8" s="18">
         <v>0.18519437566666666</v>
       </c>
-      <c r="K8" s="19">
+      <c r="K8" s="18">
         <v>0.58087119733333337</v>
       </c>
     </row>
-    <row r="9" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A9">
         <v>23</v>
       </c>
@@ -7730,7 +7726,7 @@
         <v>1.5549999999999999</v>
       </c>
     </row>
-    <row r="10" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A10">
         <v>26</v>
       </c>
@@ -7744,7 +7740,7 @@
         <v>1.0933333333333333</v>
       </c>
     </row>
-    <row r="11" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A11">
         <v>28</v>
       </c>
@@ -7758,53 +7754,53 @@
         <v>0.61166666666666669</v>
       </c>
     </row>
-    <row r="13" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="H13" s="18"/>
-      <c r="I13" s="18"/>
-      <c r="J13" s="18"/>
-      <c r="K13" s="18"/>
-      <c r="L13" s="18"/>
-      <c r="M13" s="18"/>
-    </row>
-    <row r="14" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="H14" s="18"/>
-      <c r="I14" s="18"/>
-      <c r="J14" s="18"/>
-      <c r="K14" s="18"/>
-      <c r="L14" s="18"/>
-      <c r="M14" s="18"/>
-    </row>
-    <row r="15" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="H15" s="18"/>
-      <c r="I15" s="18"/>
-      <c r="J15" s="18"/>
-      <c r="K15" s="18"/>
-      <c r="L15" s="18"/>
-      <c r="M15" s="18"/>
-    </row>
-    <row r="16" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="H16" s="18"/>
-      <c r="I16" s="18"/>
-      <c r="J16" s="18"/>
-      <c r="K16" s="18"/>
-      <c r="L16" s="18"/>
-      <c r="M16" s="18"/>
-    </row>
-    <row r="17" spans="8:13" x14ac:dyDescent="0.25">
-      <c r="H17" s="18"/>
-      <c r="I17" s="18"/>
-      <c r="J17" s="18"/>
-      <c r="K17" s="18"/>
-      <c r="L17" s="18"/>
-      <c r="M17" s="18"/>
-    </row>
-    <row r="18" spans="8:13" x14ac:dyDescent="0.25">
-      <c r="H18" s="18"/>
-      <c r="I18" s="18"/>
-      <c r="J18" s="18"/>
-      <c r="K18" s="18"/>
-      <c r="L18" s="18"/>
-      <c r="M18" s="18"/>
+    <row r="13" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="H13" s="17"/>
+      <c r="I13" s="17"/>
+      <c r="J13" s="17"/>
+      <c r="K13" s="17"/>
+      <c r="L13" s="17"/>
+      <c r="M13" s="17"/>
+    </row>
+    <row r="14" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="H14" s="17"/>
+      <c r="I14" s="17"/>
+      <c r="J14" s="17"/>
+      <c r="K14" s="17"/>
+      <c r="L14" s="17"/>
+      <c r="M14" s="17"/>
+    </row>
+    <row r="15" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="H15" s="17"/>
+      <c r="I15" s="17"/>
+      <c r="J15" s="17"/>
+      <c r="K15" s="17"/>
+      <c r="L15" s="17"/>
+      <c r="M15" s="17"/>
+    </row>
+    <row r="16" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="H16" s="17"/>
+      <c r="I16" s="17"/>
+      <c r="J16" s="17"/>
+      <c r="K16" s="17"/>
+      <c r="L16" s="17"/>
+      <c r="M16" s="17"/>
+    </row>
+    <row r="17" spans="8:13" x14ac:dyDescent="0.35">
+      <c r="H17" s="17"/>
+      <c r="I17" s="17"/>
+      <c r="J17" s="17"/>
+      <c r="K17" s="17"/>
+      <c r="L17" s="17"/>
+      <c r="M17" s="17"/>
+    </row>
+    <row r="18" spans="8:13" x14ac:dyDescent="0.35">
+      <c r="H18" s="17"/>
+      <c r="I18" s="17"/>
+      <c r="J18" s="17"/>
+      <c r="K18" s="17"/>
+      <c r="L18" s="17"/>
+      <c r="M18" s="17"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -7820,16 +7816,16 @@
       <selection activeCell="G3" sqref="G3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A1" s="16" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B2" t="s">
         <v>8</v>
@@ -7841,28 +7837,28 @@
         <v>10</v>
       </c>
       <c r="E2" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="F2" t="s">
+        <v>47</v>
+      </c>
+      <c r="G2" t="s">
         <v>48</v>
       </c>
-      <c r="G2" t="s">
+      <c r="H2" t="s">
         <v>49</v>
       </c>
-      <c r="H2" t="s">
-        <v>50</v>
-      </c>
       <c r="I2" t="s">
+        <v>44</v>
+      </c>
+      <c r="J2" t="s">
+        <v>46</v>
+      </c>
+      <c r="K2" t="s">
         <v>45</v>
       </c>
-      <c r="J2" t="s">
-        <v>47</v>
-      </c>
-      <c r="K2" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
+    </row>
+    <row r="3" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A3">
         <v>0</v>
       </c>
@@ -7897,7 +7893,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A4">
         <v>4.5</v>
       </c>
@@ -7932,7 +7928,7 @@
         <v>1.8986966135000001</v>
       </c>
     </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A5">
         <v>8.5</v>
       </c>
@@ -7967,7 +7963,7 @@
         <v>1.4777729930000001</v>
       </c>
     </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A6">
         <v>12.5</v>
       </c>
@@ -8002,7 +7998,7 @@
         <v>0.20823276374999999</v>
       </c>
     </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A7">
         <v>15.5</v>
       </c>
@@ -8037,7 +8033,7 @@
         <v>8.1622807700000008E-2</v>
       </c>
     </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A8">
         <v>17.5</v>
       </c>
@@ -8072,7 +8068,7 @@
         <v>0.10448807</v>
       </c>
     </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A9">
         <v>23</v>
       </c>
@@ -8086,7 +8082,7 @@
         <v>0.17499999999999999</v>
       </c>
     </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A10">
         <v>26</v>
       </c>
@@ -8100,7 +8096,7 @@
         <v>0.14499999999999999</v>
       </c>
     </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A11">
         <v>28</v>
       </c>
@@ -8127,22 +8123,22 @@
       <selection activeCell="W75" sqref="W75"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="12.5703125"/>
-    <col min="2" max="7" width="12.42578125" style="5"/>
-    <col min="8" max="8" width="18.85546875" style="5" bestFit="1" customWidth="1"/>
-    <col min="9" max="14" width="12.42578125" style="5"/>
-    <col min="15" max="15" width="18.5703125" style="5" bestFit="1" customWidth="1"/>
-    <col min="17" max="20" width="12.5703125"/>
+    <col min="1" max="1" width="12.54296875"/>
+    <col min="2" max="7" width="12.453125" style="5"/>
+    <col min="8" max="8" width="18.81640625" style="5" bestFit="1" customWidth="1"/>
+    <col min="9" max="14" width="12.453125" style="5"/>
+    <col min="15" max="15" width="18.54296875" style="5" bestFit="1" customWidth="1"/>
+    <col min="17" max="20" width="12.54296875"/>
     <col min="21" max="21" width="14" bestFit="1" customWidth="1"/>
-    <col min="22" max="22" width="18.28515625" bestFit="1" customWidth="1"/>
-    <col min="23" max="28" width="12.5703125"/>
-    <col min="29" max="29" width="21.7109375" bestFit="1" customWidth="1"/>
-    <col min="30" max="30" width="12.5703125"/>
+    <col min="22" max="22" width="18.26953125" bestFit="1" customWidth="1"/>
+    <col min="23" max="28" width="12.54296875"/>
+    <col min="29" max="29" width="21.7265625" bestFit="1" customWidth="1"/>
+    <col min="30" max="30" width="12.54296875"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:30" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:30" ht="16" x14ac:dyDescent="0.4">
       <c r="A1" s="3" t="s">
         <v>14</v>
       </c>
@@ -8175,7 +8171,7 @@
       <c r="AC1" s="3"/>
       <c r="AD1" s="3"/>
     </row>
-    <row r="2" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:30" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>1</v>
       </c>
@@ -8198,7 +8194,7 @@
         <v>7</v>
       </c>
       <c r="H2" s="15" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="I2" s="5" t="s">
         <v>8</v>
@@ -8219,52 +8215,52 @@
         <v>13</v>
       </c>
       <c r="O2" s="15" t="s">
+        <v>38</v>
+      </c>
+      <c r="P2" t="s">
+        <v>47</v>
+      </c>
+      <c r="Q2" t="s">
+        <v>48</v>
+      </c>
+      <c r="R2" t="s">
+        <v>49</v>
+      </c>
+      <c r="S2" t="s">
+        <v>50</v>
+      </c>
+      <c r="T2" t="s">
+        <v>51</v>
+      </c>
+      <c r="U2" t="s">
+        <v>52</v>
+      </c>
+      <c r="V2" s="16" t="s">
         <v>39</v>
       </c>
-      <c r="P2" t="s">
-        <v>48</v>
-      </c>
-      <c r="Q2" t="s">
-        <v>49</v>
-      </c>
-      <c r="R2" t="s">
-        <v>50</v>
-      </c>
-      <c r="S2" t="s">
-        <v>51</v>
-      </c>
-      <c r="T2" t="s">
-        <v>52</v>
-      </c>
-      <c r="U2" t="s">
+      <c r="W2" t="s">
+        <v>44</v>
+      </c>
+      <c r="X2" t="s">
+        <v>46</v>
+      </c>
+      <c r="Y2" t="s">
+        <v>45</v>
+      </c>
+      <c r="Z2" t="s">
         <v>53</v>
       </c>
-      <c r="V2" s="16" t="s">
+      <c r="AA2" t="s">
+        <v>54</v>
+      </c>
+      <c r="AB2" t="s">
+        <v>55</v>
+      </c>
+      <c r="AC2" s="16" t="s">
         <v>40</v>
       </c>
-      <c r="W2" t="s">
-        <v>45</v>
-      </c>
-      <c r="X2" t="s">
-        <v>47</v>
-      </c>
-      <c r="Y2" t="s">
-        <v>46</v>
-      </c>
-      <c r="Z2" t="s">
-        <v>54</v>
-      </c>
-      <c r="AA2" t="s">
-        <v>55</v>
-      </c>
-      <c r="AB2" t="s">
-        <v>56</v>
-      </c>
-      <c r="AC2" s="16" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="3" spans="1:30" x14ac:dyDescent="0.25">
+    </row>
+    <row r="3" spans="1:30" x14ac:dyDescent="0.35">
       <c r="A3">
         <v>0.5</v>
       </c>
@@ -8357,7 +8353,7 @@
         <v>1.4374999999999905</v>
       </c>
     </row>
-    <row r="4" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:30" x14ac:dyDescent="0.35">
       <c r="A4">
         <v>1</v>
       </c>
@@ -8402,7 +8398,7 @@
         <v>4.0083333333333551</v>
       </c>
       <c r="O4" s="6">
-        <f t="shared" ref="O4:O59" si="1">AVERAGE(I4:N4)</f>
+        <f t="shared" ref="O4:O58" si="1">AVERAGE(I4:N4)</f>
         <v>0.77083333333334281</v>
       </c>
       <c r="P4" s="6">
@@ -8450,7 +8446,7 @@
         <v>1.124999999999994</v>
       </c>
     </row>
-    <row r="5" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:30" x14ac:dyDescent="0.35">
       <c r="A5">
         <v>1.5</v>
       </c>
@@ -8543,7 +8539,7 @@
         <v>6.2499999999996586E-2</v>
       </c>
     </row>
-    <row r="6" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:30" x14ac:dyDescent="0.35">
       <c r="A6">
         <v>2</v>
       </c>
@@ -8636,7 +8632,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:30" x14ac:dyDescent="0.35">
       <c r="A7">
         <v>2.5</v>
       </c>
@@ -8729,7 +8725,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:30" x14ac:dyDescent="0.35">
       <c r="A8">
         <v>3</v>
       </c>
@@ -8822,7 +8818,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:30" x14ac:dyDescent="0.35">
       <c r="A9">
         <v>3.5</v>
       </c>
@@ -8915,7 +8911,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:30" x14ac:dyDescent="0.35">
       <c r="A10">
         <v>4</v>
       </c>
@@ -9008,7 +9004,7 @@
         <v>6.2499999999996586E-2</v>
       </c>
     </row>
-    <row r="11" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:30" x14ac:dyDescent="0.35">
       <c r="A11">
         <v>4.5</v>
       </c>
@@ -9101,7 +9097,7 @@
         <v>0.31249999999999684</v>
       </c>
     </row>
-    <row r="12" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:30" x14ac:dyDescent="0.35">
       <c r="A12">
         <v>5</v>
       </c>
@@ -9194,7 +9190,7 @@
         <v>5.3749999999999938</v>
       </c>
     </row>
-    <row r="13" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:30" x14ac:dyDescent="0.35">
       <c r="A13">
         <v>5.5</v>
       </c>
@@ -9287,7 +9283,7 @@
         <v>18.749999999999989</v>
       </c>
     </row>
-    <row r="14" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:30" x14ac:dyDescent="0.35">
       <c r="A14">
         <v>6</v>
       </c>
@@ -9380,7 +9376,7 @@
         <v>21.249999999999989</v>
       </c>
     </row>
-    <row r="15" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:30" x14ac:dyDescent="0.35">
       <c r="A15">
         <v>6.5</v>
       </c>
@@ -9473,7 +9469,7 @@
         <v>19.749999999999993</v>
       </c>
     </row>
-    <row r="16" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:30" x14ac:dyDescent="0.35">
       <c r="A16">
         <v>7</v>
       </c>
@@ -9566,7 +9562,7 @@
         <v>21.624999999999989</v>
       </c>
     </row>
-    <row r="17" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:29" x14ac:dyDescent="0.35">
       <c r="A17">
         <v>7.5</v>
       </c>
@@ -9659,7 +9655,7 @@
         <v>21.312499999999989</v>
       </c>
     </row>
-    <row r="18" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:29" x14ac:dyDescent="0.35">
       <c r="A18">
         <v>8</v>
       </c>
@@ -9752,7 +9748,7 @@
         <v>31.125</v>
       </c>
     </row>
-    <row r="19" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:29" x14ac:dyDescent="0.35">
       <c r="A19">
         <v>8.5</v>
       </c>
@@ -9845,7 +9841,7 @@
         <v>42.374999999999972</v>
       </c>
     </row>
-    <row r="20" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:29" x14ac:dyDescent="0.35">
       <c r="A20">
         <v>9</v>
       </c>
@@ -9938,7 +9934,7 @@
         <v>55.874999999999979</v>
       </c>
     </row>
-    <row r="21" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:29" x14ac:dyDescent="0.35">
       <c r="A21">
         <v>9.5</v>
       </c>
@@ -10031,7 +10027,7 @@
         <v>69.374999999999986</v>
       </c>
     </row>
-    <row r="22" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:29" x14ac:dyDescent="0.35">
       <c r="A22">
         <v>10</v>
       </c>
@@ -10124,7 +10120,7 @@
         <v>83.624999999999986</v>
       </c>
     </row>
-    <row r="23" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:29" x14ac:dyDescent="0.35">
       <c r="A23">
         <v>10.5</v>
       </c>
@@ -10217,7 +10213,7 @@
         <v>98.874999999999986</v>
       </c>
     </row>
-    <row r="24" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:29" x14ac:dyDescent="0.35">
       <c r="A24">
         <v>11</v>
       </c>
@@ -10310,7 +10306,7 @@
         <v>109.62499999999999</v>
       </c>
     </row>
-    <row r="25" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:29" x14ac:dyDescent="0.35">
       <c r="A25">
         <v>11.5</v>
       </c>
@@ -10403,7 +10399,7 @@
         <v>115.12499999999999</v>
       </c>
     </row>
-    <row r="26" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:29" x14ac:dyDescent="0.35">
       <c r="A26">
         <v>12</v>
       </c>
@@ -10496,7 +10492,7 @@
         <v>118.375</v>
       </c>
     </row>
-    <row r="27" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:29" x14ac:dyDescent="0.35">
       <c r="A27">
         <v>12.5</v>
       </c>
@@ -10589,7 +10585,7 @@
         <v>122.375</v>
       </c>
     </row>
-    <row r="28" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:29" x14ac:dyDescent="0.35">
       <c r="A28">
         <v>13</v>
       </c>
@@ -10682,7 +10678,7 @@
         <v>127.875</v>
       </c>
     </row>
-    <row r="29" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:29" x14ac:dyDescent="0.35">
       <c r="A29">
         <v>13.5</v>
       </c>
@@ -10775,7 +10771,7 @@
         <v>136.375</v>
       </c>
     </row>
-    <row r="30" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:29" x14ac:dyDescent="0.35">
       <c r="A30">
         <v>14</v>
       </c>
@@ -10868,7 +10864,7 @@
         <v>146.37499999999997</v>
       </c>
     </row>
-    <row r="31" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:29" x14ac:dyDescent="0.35">
       <c r="A31">
         <v>14.5</v>
       </c>
@@ -10961,7 +10957,7 @@
         <v>160.125</v>
       </c>
     </row>
-    <row r="32" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:29" x14ac:dyDescent="0.35">
       <c r="A32">
         <v>15</v>
       </c>
@@ -11054,7 +11050,7 @@
         <v>175.125</v>
       </c>
     </row>
-    <row r="33" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:29" x14ac:dyDescent="0.35">
       <c r="A33">
         <v>15.5</v>
       </c>
@@ -11147,7 +11143,7 @@
         <v>191.625</v>
       </c>
     </row>
-    <row r="34" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:29" x14ac:dyDescent="0.35">
       <c r="A34">
         <v>16</v>
       </c>
@@ -11240,7 +11236,7 @@
         <v>211.125</v>
       </c>
     </row>
-    <row r="35" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:29" x14ac:dyDescent="0.35">
       <c r="A35">
         <v>16.5</v>
       </c>
@@ -11333,7 +11329,7 @@
         <v>231.875</v>
       </c>
     </row>
-    <row r="36" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:29" x14ac:dyDescent="0.35">
       <c r="A36">
         <v>17</v>
       </c>
@@ -11426,7 +11422,7 @@
         <v>255.12499999999997</v>
       </c>
     </row>
-    <row r="37" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:29" x14ac:dyDescent="0.35">
       <c r="A37">
         <v>17.5</v>
       </c>
@@ -11519,7 +11515,7 @@
         <v>278.625</v>
       </c>
     </row>
-    <row r="38" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:29" x14ac:dyDescent="0.35">
       <c r="A38">
         <v>18</v>
       </c>
@@ -11612,7 +11608,7 @@
         <v>294.375</v>
       </c>
     </row>
-    <row r="39" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:29" x14ac:dyDescent="0.35">
       <c r="A39">
         <v>18.5</v>
       </c>
@@ -11705,7 +11701,7 @@
         <v>295.375</v>
       </c>
     </row>
-    <row r="40" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:29" x14ac:dyDescent="0.35">
       <c r="A40">
         <v>19</v>
       </c>
@@ -11798,7 +11794,7 @@
         <v>292.875</v>
       </c>
     </row>
-    <row r="41" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:29" x14ac:dyDescent="0.35">
       <c r="A41">
         <v>19.5</v>
       </c>
@@ -11891,7 +11887,7 @@
         <v>289.875</v>
       </c>
     </row>
-    <row r="42" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:29" x14ac:dyDescent="0.35">
       <c r="A42">
         <v>20</v>
       </c>
@@ -11984,7 +11980,7 @@
         <v>286.875</v>
       </c>
     </row>
-    <row r="43" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:29" x14ac:dyDescent="0.35">
       <c r="A43">
         <v>20.5</v>
       </c>
@@ -12077,7 +12073,7 @@
         <v>285.875</v>
       </c>
     </row>
-    <row r="44" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:29" x14ac:dyDescent="0.35">
       <c r="A44">
         <v>21</v>
       </c>
@@ -12170,7 +12166,7 @@
         <v>284.125</v>
       </c>
     </row>
-    <row r="45" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:29" x14ac:dyDescent="0.35">
       <c r="A45">
         <v>21.5</v>
       </c>
@@ -12263,7 +12259,7 @@
         <v>282.12499999999994</v>
       </c>
     </row>
-    <row r="46" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:29" x14ac:dyDescent="0.35">
       <c r="A46">
         <v>22</v>
       </c>
@@ -12356,7 +12352,7 @@
         <v>280.37499999999994</v>
       </c>
     </row>
-    <row r="47" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:29" x14ac:dyDescent="0.35">
       <c r="A47">
         <v>22.5</v>
       </c>
@@ -12449,7 +12445,7 @@
         <v>279.125</v>
       </c>
     </row>
-    <row r="48" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:29" x14ac:dyDescent="0.35">
       <c r="A48">
         <v>23</v>
       </c>
@@ -12542,7 +12538,7 @@
         <v>278.12499999999994</v>
       </c>
     </row>
-    <row r="49" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:29" x14ac:dyDescent="0.35">
       <c r="A49">
         <v>23.5</v>
       </c>
@@ -12635,7 +12631,7 @@
         <v>278.625</v>
       </c>
     </row>
-    <row r="50" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:29" x14ac:dyDescent="0.35">
       <c r="A50">
         <v>24</v>
       </c>
@@ -12728,7 +12724,7 @@
         <v>276.87499999999994</v>
       </c>
     </row>
-    <row r="51" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:29" x14ac:dyDescent="0.35">
       <c r="A51">
         <v>24.5</v>
       </c>
@@ -12821,7 +12817,7 @@
         <v>276.125</v>
       </c>
     </row>
-    <row r="52" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:29" x14ac:dyDescent="0.35">
       <c r="A52">
         <v>25</v>
       </c>
@@ -12914,7 +12910,7 @@
         <v>276.625</v>
       </c>
     </row>
-    <row r="53" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:29" x14ac:dyDescent="0.35">
       <c r="A53">
         <v>25.5</v>
       </c>
@@ -13007,7 +13003,7 @@
         <v>274.12499999999994</v>
       </c>
     </row>
-    <row r="54" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:29" x14ac:dyDescent="0.35">
       <c r="A54">
         <v>26</v>
       </c>
@@ -13100,7 +13096,7 @@
         <v>272.62499999999994</v>
       </c>
     </row>
-    <row r="55" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:29" x14ac:dyDescent="0.35">
       <c r="A55">
         <v>26.5</v>
       </c>
@@ -13193,7 +13189,7 @@
         <v>271.37499999999994</v>
       </c>
     </row>
-    <row r="56" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:29" x14ac:dyDescent="0.35">
       <c r="A56">
         <v>27</v>
       </c>
@@ -13286,7 +13282,7 @@
         <v>271.12499999999994</v>
       </c>
     </row>
-    <row r="57" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:29" x14ac:dyDescent="0.35">
       <c r="A57">
         <v>27.5</v>
       </c>
@@ -13379,7 +13375,7 @@
         <v>271.12499999999994</v>
       </c>
     </row>
-    <row r="58" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:29" x14ac:dyDescent="0.35">
       <c r="A58">
         <v>28</v>
       </c>
@@ -13472,10 +13468,10 @@
         <v>270.12499999999994</v>
       </c>
     </row>
-    <row r="59" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:29" x14ac:dyDescent="0.35">
       <c r="O59" s="6"/>
     </row>
-    <row r="60" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:29" x14ac:dyDescent="0.35">
       <c r="B60"/>
       <c r="C60"/>
       <c r="D60"/>
@@ -13491,7 +13487,7 @@
       <c r="N60"/>
       <c r="O60"/>
     </row>
-    <row r="61" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:29" x14ac:dyDescent="0.35">
       <c r="B61"/>
       <c r="C61"/>
       <c r="D61"/>
@@ -13507,7 +13503,7 @@
       <c r="N61"/>
       <c r="O61"/>
     </row>
-    <row r="62" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:29" x14ac:dyDescent="0.35">
       <c r="B62"/>
       <c r="C62"/>
       <c r="D62"/>
@@ -13523,7 +13519,7 @@
       <c r="N62"/>
       <c r="O62"/>
     </row>
-    <row r="63" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:29" x14ac:dyDescent="0.35">
       <c r="B63"/>
       <c r="C63"/>
       <c r="D63"/>
@@ -13539,7 +13535,7 @@
       <c r="N63"/>
       <c r="O63"/>
     </row>
-    <row r="64" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:29" x14ac:dyDescent="0.35">
       <c r="B64"/>
       <c r="C64"/>
       <c r="D64"/>
@@ -13555,86 +13551,86 @@
       <c r="N64"/>
       <c r="O64"/>
     </row>
-    <row r="65" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="66" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="67" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="68" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="69" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="70" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="71" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="72" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="73" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="74" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="75" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="76" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="77" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="78" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="79" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="80" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="81" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="82" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="83" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="84" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="85" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="86" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="87" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="88" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="89" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="90" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="91" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="92" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="93" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="94" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="95" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="96" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="97" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="98" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="99" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="100" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="101" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="102" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="103" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="104" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="105" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="106" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="107" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="108" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="109" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="110" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="111" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="112" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="113" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="114" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="115" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="116" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="117" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="118" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="119" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="120" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="121" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="122" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="123" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="124" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="125" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="126" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="127" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="128" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="129" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="130" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="131" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="132" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="133" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="134" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="135" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="136" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="137" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="138" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="139" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="140" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="141" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="142" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="143" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="144" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="65" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="66" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="67" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="68" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="69" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="70" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="71" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="72" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="73" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="74" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="75" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="76" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="77" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="78" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="79" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="80" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="81" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="82" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="83" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="84" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="85" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="86" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="87" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="88" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="89" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="90" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="91" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="92" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="93" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="94" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="95" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="96" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="97" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="98" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="99" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="100" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="101" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="102" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="103" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="104" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="105" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="106" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="107" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="108" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="109" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="110" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="111" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="112" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="113" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="114" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="115" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="116" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="117" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="118" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="119" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="120" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="121" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="122" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="123" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="124" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="125" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="126" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="127" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="128" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="129" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="130" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="131" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="132" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="133" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="134" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="135" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="136" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="137" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="138" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="139" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="140" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="141" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="142" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="143" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="144" customFormat="1" x14ac:dyDescent="0.35"/>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -13642,25 +13638,25 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BBF2D4E9-7129-477A-86E2-156B785AADAF}">
-  <dimension ref="A1:R144"/>
+  <dimension ref="A1:Q144"/>
   <sheetViews>
     <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
       <selection activeCell="E56" sqref="E56"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="12.5703125"/>
-    <col min="2" max="4" width="12.42578125" style="5"/>
-    <col min="5" max="5" width="15.85546875" style="5" bestFit="1" customWidth="1"/>
-    <col min="6" max="8" width="12.42578125" style="5"/>
-    <col min="9" max="9" width="15.42578125" style="5" bestFit="1" customWidth="1"/>
-    <col min="10" max="12" width="12.5703125"/>
-    <col min="13" max="13" width="23.140625" bestFit="1" customWidth="1"/>
-    <col min="14" max="16" width="12.5703125"/>
+    <col min="1" max="1" width="12.54296875"/>
+    <col min="2" max="4" width="12.453125" style="5"/>
+    <col min="5" max="5" width="15.81640625" style="5" bestFit="1" customWidth="1"/>
+    <col min="6" max="8" width="12.453125" style="5"/>
+    <col min="9" max="9" width="15.453125" style="5" bestFit="1" customWidth="1"/>
+    <col min="10" max="12" width="12.54296875"/>
+    <col min="13" max="13" width="23.1796875" bestFit="1" customWidth="1"/>
+    <col min="14" max="16" width="12.54296875"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:18" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:17" ht="16" x14ac:dyDescent="0.4">
       <c r="A1" s="3" t="s">
         <v>15</v>
       </c>
@@ -13680,7 +13676,7 @@
       <c r="O1" s="3"/>
       <c r="P1" s="3"/>
     </row>
-    <row r="2" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A2" s="10" t="s">
         <v>30</v>
       </c>
@@ -13694,7 +13690,7 @@
         <v>18</v>
       </c>
       <c r="E2" s="15" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="F2" s="5" t="s">
         <v>19</v>
@@ -13706,7 +13702,7 @@
         <v>21</v>
       </c>
       <c r="I2" s="15" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="J2" t="s">
         <v>31</v>
@@ -13718,7 +13714,7 @@
         <v>33</v>
       </c>
       <c r="M2" s="16" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="N2" t="s">
         <v>34</v>
@@ -13730,11 +13726,10 @@
         <v>36</v>
       </c>
       <c r="Q2" s="16" t="s">
-        <v>41</v>
-      </c>
-      <c r="R2" s="17"/>
-    </row>
-    <row r="3" spans="1:18" x14ac:dyDescent="0.25">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="3" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A3">
         <v>0.5</v>
       </c>
@@ -13791,7 +13786,7 @@
         <v>-0.21385845999999997</v>
       </c>
     </row>
-    <row r="4" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A4">
         <v>1</v>
       </c>
@@ -13848,7 +13843,7 @@
         <v>-0.22742141814285721</v>
       </c>
     </row>
-    <row r="5" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A5">
         <v>1.5</v>
       </c>
@@ -13905,7 +13900,7 @@
         <v>0.11439124816666661</v>
       </c>
     </row>
-    <row r="6" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A6">
         <v>2</v>
       </c>
@@ -13962,7 +13957,7 @@
         <v>0.4631693907380951</v>
       </c>
     </row>
-    <row r="7" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A7">
         <v>2.5</v>
       </c>
@@ -14019,7 +14014,7 @@
         <v>1.1520892362857138</v>
       </c>
     </row>
-    <row r="8" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A8">
         <v>3</v>
       </c>
@@ -14076,7 +14071,7 @@
         <v>1.9955135086785709</v>
       </c>
     </row>
-    <row r="9" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A9">
         <v>3.5</v>
       </c>
@@ -14133,7 +14128,7 @@
         <v>4.0233845559999981</v>
       </c>
     </row>
-    <row r="10" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A10">
         <v>4</v>
       </c>
@@ -14190,7 +14185,7 @@
         <v>5.7449334324999981</v>
       </c>
     </row>
-    <row r="11" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A11">
         <v>4.5</v>
       </c>
@@ -14247,7 +14242,7 @@
         <v>7.598579886714286</v>
       </c>
     </row>
-    <row r="12" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A12">
         <v>5</v>
       </c>
@@ -14304,7 +14299,7 @@
         <v>9.908700402202383</v>
       </c>
     </row>
-    <row r="13" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A13">
         <v>5.5</v>
       </c>
@@ -14361,7 +14356,7 @@
         <v>12.93955016828572</v>
       </c>
     </row>
-    <row r="14" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A14">
         <v>6</v>
       </c>
@@ -14418,7 +14413,7 @@
         <v>16.444045934750012</v>
       </c>
     </row>
-    <row r="15" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A15">
         <v>6.5</v>
       </c>
@@ -14475,7 +14470,7 @@
         <v>20.638727251904779</v>
       </c>
     </row>
-    <row r="16" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A16">
         <v>7</v>
       </c>
@@ -14532,7 +14527,7 @@
         <v>25.39078373190479</v>
       </c>
     </row>
-    <row r="17" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A17">
         <v>7.5</v>
       </c>
@@ -14589,7 +14584,7 @@
         <v>31.027388036666697</v>
       </c>
     </row>
-    <row r="18" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A18">
         <v>8</v>
       </c>
@@ -14646,7 +14641,7 @@
         <v>37.106020603214326</v>
       </c>
     </row>
-    <row r="19" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A19">
         <v>8.5</v>
       </c>
@@ -14703,7 +14698,7 @@
         <v>44.252532391428623</v>
       </c>
     </row>
-    <row r="20" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A20">
         <v>9</v>
       </c>
@@ -14760,7 +14755,7 @@
         <v>52.278144364166735</v>
       </c>
     </row>
-    <row r="21" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A21">
         <v>9.5</v>
       </c>
@@ -14817,7 +14812,7 @@
         <v>61.723859052381044</v>
       </c>
     </row>
-    <row r="22" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A22">
         <v>10</v>
       </c>
@@ -14874,7 +14869,7 @@
         <v>72.942246405238208</v>
       </c>
     </row>
-    <row r="23" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A23">
         <v>10.5</v>
       </c>
@@ -14931,7 +14926,7 @@
         <v>85.110925019523947</v>
       </c>
     </row>
-    <row r="24" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A24">
         <v>11</v>
       </c>
@@ -14988,7 +14983,7 @@
         <v>97.608073041666827</v>
       </c>
     </row>
-    <row r="25" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A25">
         <v>11.5</v>
       </c>
@@ -15045,7 +15040,7 @@
         <v>109.69754447476207</v>
       </c>
     </row>
-    <row r="26" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A26">
         <v>12</v>
       </c>
@@ -15102,7 +15097,7 @@
         <v>121.95977381964299</v>
       </c>
     </row>
-    <row r="27" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A27">
         <v>12.5</v>
       </c>
@@ -15159,7 +15154,7 @@
         <v>133.87238508095257</v>
       </c>
     </row>
-    <row r="28" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A28">
         <v>13</v>
       </c>
@@ -15216,7 +15211,7 @@
         <v>146.08774197738114</v>
       </c>
     </row>
-    <row r="29" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A29">
         <v>13.5</v>
       </c>
@@ -15273,7 +15268,7 @@
         <v>158.41650850238116</v>
       </c>
     </row>
-    <row r="30" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A30">
         <v>14</v>
       </c>
@@ -15330,7 +15325,7 @@
         <v>170.91917976309546</v>
       </c>
     </row>
-    <row r="31" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A31">
         <v>14.5</v>
       </c>
@@ -15387,7 +15382,7 @@
         <v>183.85954896666689</v>
       </c>
     </row>
-    <row r="32" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A32">
         <v>15</v>
       </c>
@@ -15444,7 +15439,7 @@
         <v>197.08026087857169</v>
       </c>
     </row>
-    <row r="33" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A33">
         <v>15.5</v>
       </c>
@@ -15501,7 +15496,7 @@
         <v>211.99122838095266</v>
       </c>
     </row>
-    <row r="34" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A34">
         <v>16</v>
       </c>
@@ -15558,7 +15553,7 @@
         <v>227.1261504130955</v>
       </c>
     </row>
-    <row r="35" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A35">
         <v>16.5</v>
       </c>
@@ -15615,7 +15610,7 @@
         <v>243.41297653333359</v>
       </c>
     </row>
-    <row r="36" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A36">
         <v>17</v>
       </c>
@@ -15672,7 +15667,7 @@
         <v>261.35487370595257</v>
       </c>
     </row>
-    <row r="37" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A37">
         <v>17.5</v>
       </c>
@@ -15729,7 +15724,7 @@
         <v>280.91125759761923</v>
       </c>
     </row>
-    <row r="38" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A38">
         <v>18</v>
       </c>
@@ -15786,7 +15781,7 @@
         <v>301.83657134166674</v>
       </c>
     </row>
-    <row r="39" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A39">
         <v>18.5</v>
       </c>
@@ -15843,7 +15838,7 @@
         <v>321.96646159523812</v>
       </c>
     </row>
-    <row r="40" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A40">
         <v>19</v>
       </c>
@@ -15900,7 +15895,7 @@
         <v>341.20011487380953</v>
       </c>
     </row>
-    <row r="41" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A41">
         <v>19.5</v>
       </c>
@@ -15957,7 +15952,7 @@
         <v>359.56309985952367</v>
       </c>
     </row>
-    <row r="42" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A42">
         <v>20</v>
       </c>
@@ -16014,7 +16009,7 @@
         <v>378.18884291666649</v>
       </c>
     </row>
-    <row r="43" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A43">
         <v>20.5</v>
       </c>
@@ -16071,7 +16066,7 @@
         <v>395.14754456190457</v>
       </c>
     </row>
-    <row r="44" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A44">
         <v>21</v>
       </c>
@@ -16128,7 +16123,7 @@
         <v>410.27749899047598</v>
       </c>
     </row>
-    <row r="45" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A45">
         <v>21.5</v>
       </c>
@@ -16185,7 +16180,7 @@
         <v>423.84135438333306</v>
       </c>
     </row>
-    <row r="46" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A46">
         <v>22</v>
       </c>
@@ -16242,7 +16237,7 @@
         <v>436.00259589285696</v>
       </c>
     </row>
-    <row r="47" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A47">
         <v>22.5</v>
       </c>
@@ -16299,7 +16294,7 @@
         <v>447.14115395714265</v>
       </c>
     </row>
-    <row r="48" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A48">
         <v>23</v>
       </c>
@@ -16356,7 +16351,7 @@
         <v>457.40536091666644</v>
       </c>
     </row>
-    <row r="49" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A49">
         <v>23.5</v>
       </c>
@@ -16413,7 +16408,7 @@
         <v>466.5461585452378</v>
       </c>
     </row>
-    <row r="50" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A50">
         <v>24</v>
       </c>
@@ -16470,7 +16465,7 @@
         <v>475.03680910714257</v>
       </c>
     </row>
-    <row r="51" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A51">
         <v>24.5</v>
       </c>
@@ -16527,7 +16522,7 @@
         <v>482.94742794285685</v>
       </c>
     </row>
-    <row r="52" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A52">
         <v>25</v>
       </c>
@@ -16584,7 +16579,7 @@
         <v>490.45740919999974</v>
       </c>
     </row>
-    <row r="53" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A53">
         <v>25.5</v>
       </c>
@@ -16641,7 +16636,7 @@
         <v>497.32838813809502</v>
       </c>
     </row>
-    <row r="54" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A54">
         <v>26</v>
       </c>
@@ -16698,7 +16693,7 @@
         <v>503.03349463809491</v>
       </c>
     </row>
-    <row r="55" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A55">
         <v>26.5</v>
       </c>
@@ -16729,7 +16724,7 @@
         <v>508.68822672380929</v>
       </c>
     </row>
-    <row r="56" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A56">
         <v>27</v>
       </c>
@@ -16760,7 +16755,7 @@
         <v>513.45149708333315</v>
       </c>
     </row>
-    <row r="57" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A57">
         <v>27.5</v>
       </c>
@@ -16791,7 +16786,7 @@
         <v>518.00753678333308</v>
       </c>
     </row>
-    <row r="58" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A58">
         <v>28</v>
       </c>
@@ -16822,7 +16817,7 @@
         <v>522.41747744880922</v>
       </c>
     </row>
-    <row r="59" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A59">
         <v>28.5</v>
       </c>
@@ -16853,7 +16848,7 @@
         <v>526.65488183333309</v>
       </c>
     </row>
-    <row r="60" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:17" x14ac:dyDescent="0.35">
       <c r="B60"/>
       <c r="C60"/>
       <c r="D60"/>
@@ -16863,7 +16858,7 @@
       <c r="H60"/>
       <c r="I60"/>
     </row>
-    <row r="61" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:17" x14ac:dyDescent="0.35">
       <c r="B61"/>
       <c r="C61"/>
       <c r="D61"/>
@@ -16873,7 +16868,7 @@
       <c r="H61"/>
       <c r="I61"/>
     </row>
-    <row r="62" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:17" x14ac:dyDescent="0.35">
       <c r="B62"/>
       <c r="C62"/>
       <c r="D62"/>
@@ -16883,7 +16878,7 @@
       <c r="H62"/>
       <c r="I62"/>
     </row>
-    <row r="63" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:17" x14ac:dyDescent="0.35">
       <c r="B63"/>
       <c r="C63"/>
       <c r="D63"/>
@@ -16893,7 +16888,7 @@
       <c r="H63"/>
       <c r="I63"/>
     </row>
-    <row r="64" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:17" x14ac:dyDescent="0.35">
       <c r="B64"/>
       <c r="C64"/>
       <c r="D64"/>
@@ -16903,86 +16898,86 @@
       <c r="H64"/>
       <c r="I64"/>
     </row>
-    <row r="65" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="66" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="67" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="68" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="69" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="70" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="71" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="72" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="73" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="74" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="75" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="76" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="77" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="78" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="79" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="80" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="81" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="82" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="83" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="84" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="85" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="86" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="87" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="88" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="89" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="90" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="91" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="92" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="93" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="94" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="95" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="96" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="97" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="98" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="99" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="100" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="101" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="102" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="103" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="104" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="105" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="106" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="107" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="108" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="109" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="110" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="111" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="112" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="113" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="114" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="115" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="116" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="117" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="118" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="119" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="120" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="121" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="122" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="123" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="124" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="125" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="126" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="127" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="128" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="129" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="130" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="131" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="132" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="133" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="134" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="135" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="136" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="137" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="138" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="139" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="140" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="141" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="142" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="143" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="144" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="65" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="66" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="67" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="68" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="69" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="70" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="71" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="72" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="73" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="74" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="75" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="76" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="77" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="78" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="79" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="80" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="81" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="82" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="83" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="84" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="85" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="86" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="87" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="88" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="89" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="90" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="91" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="92" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="93" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="94" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="95" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="96" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="97" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="98" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="99" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="100" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="101" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="102" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="103" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="104" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="105" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="106" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="107" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="108" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="109" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="110" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="111" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="112" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="113" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="114" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="115" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="116" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="117" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="118" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="119" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="120" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="121" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="122" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="123" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="124" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="125" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="126" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="127" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="128" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="129" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="130" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="131" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="132" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="133" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="134" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="135" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="136" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="137" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="138" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="139" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="140" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="141" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="142" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="143" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="144" customFormat="1" x14ac:dyDescent="0.35"/>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -16992,24 +16987,24 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BAA9ADE4-95E1-451A-8686-8E2AE4EC2460}">
   <dimension ref="A1:R144"/>
   <sheetViews>
-    <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="Q20" sqref="Q20"/>
+    <sheetView tabSelected="1" topLeftCell="A15" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="M33" sqref="M33"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="12.5703125"/>
-    <col min="2" max="4" width="12.42578125" style="5"/>
-    <col min="5" max="5" width="15.85546875" style="5" bestFit="1" customWidth="1"/>
-    <col min="6" max="8" width="12.42578125" style="5"/>
-    <col min="9" max="9" width="15.42578125" style="5" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="12.5703125"/>
-    <col min="12" max="12" width="12.42578125" style="5"/>
-    <col min="13" max="13" width="23.140625" style="5" bestFit="1" customWidth="1"/>
-    <col min="14" max="18" width="12.42578125" style="5"/>
+    <col min="1" max="1" width="12.54296875"/>
+    <col min="2" max="4" width="12.453125" style="5"/>
+    <col min="5" max="5" width="15.81640625" style="5" bestFit="1" customWidth="1"/>
+    <col min="6" max="8" width="12.453125" style="5"/>
+    <col min="9" max="9" width="15.453125" style="5" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="12.54296875"/>
+    <col min="12" max="12" width="12.453125" style="5"/>
+    <col min="13" max="13" width="23.1796875" style="5" bestFit="1" customWidth="1"/>
+    <col min="14" max="18" width="12.453125" style="5"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:18" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:18" ht="16" x14ac:dyDescent="0.4">
       <c r="A1" s="3" t="s">
         <v>22</v>
       </c>
@@ -17030,7 +17025,7 @@
       <c r="Q1" s="4"/>
       <c r="R1" s="4"/>
     </row>
-    <row r="2" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A2" s="10" t="s">
         <v>30</v>
       </c>
@@ -17044,7 +17039,7 @@
         <v>18</v>
       </c>
       <c r="E2" s="15" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="F2" s="5" t="s">
         <v>19</v>
@@ -17056,7 +17051,7 @@
         <v>21</v>
       </c>
       <c r="I2" s="15" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="J2" s="5" t="s">
         <v>31</v>
@@ -17068,7 +17063,7 @@
         <v>33</v>
       </c>
       <c r="M2" s="15" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="N2" s="5" t="s">
         <v>34</v>
@@ -17080,10 +17075,10 @@
         <v>36</v>
       </c>
       <c r="Q2" s="5" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="3" spans="1:18" x14ac:dyDescent="0.25">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="3" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A3">
         <v>0.5</v>
       </c>
@@ -17140,7 +17135,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A4">
         <v>1</v>
       </c>
@@ -17193,11 +17188,11 @@
         <v>0.71110343545310417</v>
       </c>
       <c r="Q4" s="5">
-        <f t="shared" ref="Q4:Q55" si="1">AVERAGE(N4:P4)</f>
+        <f t="shared" ref="Q4:Q53" si="1">AVERAGE(N4:P4)</f>
         <v>0.23703447848436807</v>
       </c>
     </row>
-    <row r="5" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A5">
         <v>1.5</v>
       </c>
@@ -17211,7 +17206,7 @@
         <v>1.0779004644204593</v>
       </c>
       <c r="E5" s="6">
-        <f t="shared" ref="E4:E54" si="2">AVERAGE(B5:D5)</f>
+        <f t="shared" ref="E5:E54" si="2">AVERAGE(B5:D5)</f>
         <v>1.2415226254566951</v>
       </c>
       <c r="F5" s="6">
@@ -17224,7 +17219,7 @@
         <v>14.268920128747496</v>
       </c>
       <c r="I5" s="6">
-        <f t="shared" ref="I4:I54" si="3">AVERAGE(F5:H5)</f>
+        <f t="shared" ref="I5:I54" si="3">AVERAGE(F5:H5)</f>
         <v>4.7563067095824989</v>
       </c>
       <c r="J5" s="6">
@@ -17254,7 +17249,7 @@
         <v>0.34017088455665573</v>
       </c>
     </row>
-    <row r="6" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A6">
         <v>2</v>
       </c>
@@ -17311,7 +17306,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A7">
         <v>2.5</v>
       </c>
@@ -17368,7 +17363,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A8">
         <v>3</v>
       </c>
@@ -17425,7 +17420,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A9">
         <v>3.5</v>
       </c>
@@ -17482,7 +17477,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A10">
         <v>4</v>
       </c>
@@ -17539,7 +17534,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A11">
         <v>4.5</v>
       </c>
@@ -17596,7 +17591,7 @@
         <v>7.210365293754202E-2</v>
       </c>
     </row>
-    <row r="12" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A12">
         <v>5</v>
       </c>
@@ -17653,7 +17648,7 @@
         <v>-8.0616235114763707E-2</v>
       </c>
     </row>
-    <row r="13" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A13">
         <v>5.5</v>
       </c>
@@ -17710,7 +17705,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A14">
         <v>6</v>
       </c>
@@ -17767,7 +17762,7 @@
         <v>0.22541700605469819</v>
       </c>
     </row>
-    <row r="15" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A15">
         <v>6.5</v>
       </c>
@@ -17824,7 +17819,7 @@
         <v>5.2243048569843262</v>
       </c>
     </row>
-    <row r="16" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A16">
         <v>7</v>
       </c>
@@ -17881,7 +17876,7 @@
         <v>-0.21417699726005271</v>
       </c>
     </row>
-    <row r="17" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A17">
         <v>7.5</v>
       </c>
@@ -17938,7 +17933,7 @@
         <v>0.23890606031557557</v>
       </c>
     </row>
-    <row r="18" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A18">
         <v>8</v>
       </c>
@@ -17995,7 +17990,7 @@
         <v>0.26359315052743948</v>
       </c>
     </row>
-    <row r="19" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A19">
         <v>8.5</v>
       </c>
@@ -18052,7 +18047,7 @@
         <v>9.9388751533123917E-2</v>
       </c>
     </row>
-    <row r="20" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A20">
         <v>9</v>
       </c>
@@ -18109,7 +18104,7 @@
         <v>0.33750903558916567</v>
       </c>
     </row>
-    <row r="21" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A21">
         <v>9.5</v>
       </c>
@@ -18166,7 +18161,7 @@
         <v>0.35699208873738542</v>
       </c>
     </row>
-    <row r="22" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A22">
         <v>10</v>
       </c>
@@ -18223,7 +18218,7 @@
         <v>0.33393554445449519</v>
       </c>
     </row>
-    <row r="23" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A23">
         <v>10.5</v>
       </c>
@@ -18280,7 +18275,7 @@
         <v>0.36015142198316658</v>
       </c>
     </row>
-    <row r="24" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A24">
         <v>11</v>
       </c>
@@ -18337,7 +18332,7 @@
         <v>0.39155247522230185</v>
       </c>
     </row>
-    <row r="25" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A25">
         <v>11.5</v>
       </c>
@@ -18394,7 +18389,7 @@
         <v>0.41059824181077209</v>
       </c>
     </row>
-    <row r="26" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A26">
         <v>12</v>
       </c>
@@ -18451,7 +18446,7 @@
         <v>0.36867891080506787</v>
       </c>
     </row>
-    <row r="27" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A27">
         <v>12.5</v>
       </c>
@@ -18508,7 +18503,7 @@
         <v>0.41234001450162799</v>
       </c>
     </row>
-    <row r="28" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A28">
         <v>13</v>
       </c>
@@ -18565,7 +18560,7 @@
         <v>0.41855343450315807</v>
       </c>
     </row>
-    <row r="29" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A29">
         <v>13.5</v>
       </c>
@@ -18622,7 +18617,7 @@
         <v>0.457706704941167</v>
       </c>
     </row>
-    <row r="30" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A30">
         <v>14</v>
       </c>
@@ -18679,7 +18674,7 @@
         <v>0.49827428989638206</v>
       </c>
     </row>
-    <row r="31" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A31">
         <v>14.5</v>
       </c>
@@ -18736,7 +18731,7 @@
         <v>0.53376848458197101</v>
       </c>
     </row>
-    <row r="32" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A32">
         <v>15</v>
       </c>
@@ -18793,7 +18788,7 @@
         <v>0.54925716798038049</v>
       </c>
     </row>
-    <row r="33" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A33">
         <v>15.5</v>
       </c>
@@ -18848,7 +18843,7 @@
         <v>0.5553082100626926</v>
       </c>
     </row>
-    <row r="34" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A34">
         <v>16</v>
       </c>
@@ -18884,9 +18879,7 @@
       <c r="K34" s="8">
         <v>9.7852820795400142E-2</v>
       </c>
-      <c r="L34" s="8" t="s">
-        <v>37</v>
-      </c>
+      <c r="L34" s="8"/>
       <c r="M34" s="6">
         <f t="shared" si="0"/>
         <v>0.28270334044791501</v>
@@ -18905,7 +18898,7 @@
         <v>0.58123318792395817</v>
       </c>
     </row>
-    <row r="35" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A35">
         <v>16.5</v>
       </c>
@@ -18962,7 +18955,7 @@
         <v>0.18169686919040687</v>
       </c>
     </row>
-    <row r="36" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A36">
         <v>17</v>
       </c>
@@ -19019,7 +19012,7 @@
         <v>0.14088184152665997</v>
       </c>
     </row>
-    <row r="37" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A37">
         <v>17.5</v>
       </c>
@@ -19076,7 +19069,7 @@
         <v>0.184165420102926</v>
       </c>
     </row>
-    <row r="38" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A38">
         <v>18</v>
       </c>
@@ -19133,7 +19126,7 @@
         <v>0.25044025623887078</v>
       </c>
     </row>
-    <row r="39" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A39">
         <v>18.5</v>
       </c>
@@ -19190,7 +19183,7 @@
         <v>0.33374054116207424</v>
       </c>
     </row>
-    <row r="40" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A40">
         <v>19</v>
       </c>
@@ -19247,7 +19240,7 @@
         <v>0.34694895513688007</v>
       </c>
     </row>
-    <row r="41" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A41">
         <v>19.5</v>
       </c>
@@ -19304,7 +19297,7 @@
         <v>-0.15044900447057855</v>
       </c>
     </row>
-    <row r="42" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A42">
         <v>20</v>
       </c>
@@ -19361,7 +19354,7 @@
         <v>-9.2057844245764242E-2</v>
       </c>
     </row>
-    <row r="43" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A43">
         <v>20.5</v>
       </c>
@@ -19418,7 +19411,7 @@
         <v>-0.17067037963969703</v>
       </c>
     </row>
-    <row r="44" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A44">
         <v>21</v>
       </c>
@@ -19475,7 +19468,7 @@
         <v>-4.9392690138745671E-2</v>
       </c>
     </row>
-    <row r="45" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A45">
         <v>21.5</v>
       </c>
@@ -19532,7 +19525,7 @@
         <v>-0.1180649915617778</v>
       </c>
     </row>
-    <row r="46" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A46">
         <v>22</v>
       </c>
@@ -19589,7 +19582,7 @@
         <v>-8.4044939044666978E-2</v>
       </c>
     </row>
-    <row r="47" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A47">
         <v>22.5</v>
       </c>
@@ -19646,7 +19639,7 @@
         <v>-3.3089179680421452E-2</v>
       </c>
     </row>
-    <row r="48" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A48">
         <v>23</v>
       </c>
@@ -19703,7 +19696,7 @@
         <v>-8.4716328376315098E-2</v>
       </c>
     </row>
-    <row r="49" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A49">
         <v>23.5</v>
       </c>
@@ -19760,7 +19753,7 @@
         <v>-1.2423439680934789E-2</v>
       </c>
     </row>
-    <row r="50" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A50">
         <v>24</v>
       </c>
@@ -19817,7 +19810,7 @@
         <v>-0.16713037763512764</v>
       </c>
     </row>
-    <row r="51" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A51">
         <v>24.5</v>
       </c>
@@ -19874,7 +19867,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="52" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A52">
         <v>25</v>
       </c>
@@ -19931,7 +19924,7 @@
         <v>-0.13637685571659988</v>
       </c>
     </row>
-    <row r="53" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A53">
         <v>25.5</v>
       </c>
@@ -19988,7 +19981,7 @@
         <v>-6.2927390015745724E-2</v>
       </c>
     </row>
-    <row r="54" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A54">
         <v>26</v>
       </c>
@@ -20045,7 +20038,7 @@
         <v>-3.9751196146820246E-2</v>
       </c>
     </row>
-    <row r="55" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A55">
         <v>26.5</v>
       </c>
@@ -20076,7 +20069,7 @@
         <v>-0.39411951271787382</v>
       </c>
     </row>
-    <row r="56" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A56">
         <v>27</v>
       </c>
@@ -20107,7 +20100,7 @@
         <v>-9.7888613831110319E-2</v>
       </c>
     </row>
-    <row r="60" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:17" x14ac:dyDescent="0.35">
       <c r="B60"/>
       <c r="C60"/>
       <c r="D60"/>
@@ -20117,7 +20110,7 @@
       <c r="H60"/>
       <c r="I60"/>
     </row>
-    <row r="61" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:17" x14ac:dyDescent="0.35">
       <c r="B61"/>
       <c r="C61"/>
       <c r="D61"/>
@@ -20127,7 +20120,7 @@
       <c r="H61"/>
       <c r="I61"/>
     </row>
-    <row r="62" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:17" x14ac:dyDescent="0.35">
       <c r="B62"/>
       <c r="C62"/>
       <c r="D62"/>
@@ -20137,7 +20130,7 @@
       <c r="H62"/>
       <c r="I62"/>
     </row>
-    <row r="63" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:17" x14ac:dyDescent="0.35">
       <c r="B63"/>
       <c r="C63"/>
       <c r="D63"/>
@@ -20147,7 +20140,7 @@
       <c r="H63"/>
       <c r="I63"/>
     </row>
-    <row r="64" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:17" x14ac:dyDescent="0.35">
       <c r="B64"/>
       <c r="C64"/>
       <c r="D64"/>
@@ -20157,7 +20150,7 @@
       <c r="H64"/>
       <c r="I64"/>
     </row>
-    <row r="65" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="65" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B65"/>
       <c r="C65"/>
       <c r="D65"/>
@@ -20167,7 +20160,7 @@
       <c r="H65"/>
       <c r="I65"/>
     </row>
-    <row r="66" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="66" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B66"/>
       <c r="C66"/>
       <c r="D66"/>
@@ -20177,7 +20170,7 @@
       <c r="H66"/>
       <c r="I66"/>
     </row>
-    <row r="67" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="67" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B67"/>
       <c r="C67"/>
       <c r="D67"/>
@@ -20187,7 +20180,7 @@
       <c r="H67"/>
       <c r="I67"/>
     </row>
-    <row r="68" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="68" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B68"/>
       <c r="C68"/>
       <c r="D68"/>
@@ -20197,7 +20190,7 @@
       <c r="H68"/>
       <c r="I68"/>
     </row>
-    <row r="69" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="69" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B69"/>
       <c r="C69"/>
       <c r="D69"/>
@@ -20207,7 +20200,7 @@
       <c r="H69"/>
       <c r="I69"/>
     </row>
-    <row r="70" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="70" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B70"/>
       <c r="C70"/>
       <c r="D70"/>
@@ -20217,7 +20210,7 @@
       <c r="H70"/>
       <c r="I70"/>
     </row>
-    <row r="71" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="71" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B71"/>
       <c r="C71"/>
       <c r="D71"/>
@@ -20227,7 +20220,7 @@
       <c r="H71"/>
       <c r="I71"/>
     </row>
-    <row r="72" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="72" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B72"/>
       <c r="C72"/>
       <c r="D72"/>
@@ -20237,7 +20230,7 @@
       <c r="H72"/>
       <c r="I72"/>
     </row>
-    <row r="73" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="73" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B73"/>
       <c r="C73"/>
       <c r="D73"/>
@@ -20247,7 +20240,7 @@
       <c r="H73"/>
       <c r="I73"/>
     </row>
-    <row r="74" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="74" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B74"/>
       <c r="C74"/>
       <c r="D74"/>
@@ -20257,7 +20250,7 @@
       <c r="H74"/>
       <c r="I74"/>
     </row>
-    <row r="75" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="75" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B75"/>
       <c r="C75"/>
       <c r="D75"/>
@@ -20267,7 +20260,7 @@
       <c r="H75"/>
       <c r="I75"/>
     </row>
-    <row r="76" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="76" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B76"/>
       <c r="C76"/>
       <c r="D76"/>
@@ -20277,7 +20270,7 @@
       <c r="H76"/>
       <c r="I76"/>
     </row>
-    <row r="77" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="77" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B77"/>
       <c r="C77"/>
       <c r="D77"/>
@@ -20287,7 +20280,7 @@
       <c r="H77"/>
       <c r="I77"/>
     </row>
-    <row r="78" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="78" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B78"/>
       <c r="C78"/>
       <c r="D78"/>
@@ -20297,7 +20290,7 @@
       <c r="H78"/>
       <c r="I78"/>
     </row>
-    <row r="79" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="79" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B79"/>
       <c r="C79"/>
       <c r="D79"/>
@@ -20307,7 +20300,7 @@
       <c r="H79"/>
       <c r="I79"/>
     </row>
-    <row r="80" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="80" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B80"/>
       <c r="C80"/>
       <c r="D80"/>
@@ -20317,7 +20310,7 @@
       <c r="H80"/>
       <c r="I80"/>
     </row>
-    <row r="81" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="81" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B81"/>
       <c r="C81"/>
       <c r="D81"/>
@@ -20327,7 +20320,7 @@
       <c r="H81"/>
       <c r="I81"/>
     </row>
-    <row r="82" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="82" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B82"/>
       <c r="C82"/>
       <c r="D82"/>
@@ -20337,7 +20330,7 @@
       <c r="H82"/>
       <c r="I82"/>
     </row>
-    <row r="83" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="83" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B83"/>
       <c r="C83"/>
       <c r="D83"/>
@@ -20347,7 +20340,7 @@
       <c r="H83"/>
       <c r="I83"/>
     </row>
-    <row r="84" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="84" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B84"/>
       <c r="C84"/>
       <c r="D84"/>
@@ -20357,7 +20350,7 @@
       <c r="H84"/>
       <c r="I84"/>
     </row>
-    <row r="85" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="85" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B85"/>
       <c r="C85"/>
       <c r="D85"/>
@@ -20367,7 +20360,7 @@
       <c r="H85"/>
       <c r="I85"/>
     </row>
-    <row r="86" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="86" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B86"/>
       <c r="C86"/>
       <c r="D86"/>
@@ -20377,7 +20370,7 @@
       <c r="H86"/>
       <c r="I86"/>
     </row>
-    <row r="87" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="87" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B87"/>
       <c r="C87"/>
       <c r="D87"/>
@@ -20387,7 +20380,7 @@
       <c r="H87"/>
       <c r="I87"/>
     </row>
-    <row r="88" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="88" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B88"/>
       <c r="C88"/>
       <c r="D88"/>
@@ -20397,7 +20390,7 @@
       <c r="H88"/>
       <c r="I88"/>
     </row>
-    <row r="89" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="89" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B89"/>
       <c r="C89"/>
       <c r="D89"/>
@@ -20407,7 +20400,7 @@
       <c r="H89"/>
       <c r="I89"/>
     </row>
-    <row r="90" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="90" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B90"/>
       <c r="C90"/>
       <c r="D90"/>
@@ -20417,7 +20410,7 @@
       <c r="H90"/>
       <c r="I90"/>
     </row>
-    <row r="91" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="91" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B91"/>
       <c r="C91"/>
       <c r="D91"/>
@@ -20427,7 +20420,7 @@
       <c r="H91"/>
       <c r="I91"/>
     </row>
-    <row r="92" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="92" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B92"/>
       <c r="C92"/>
       <c r="D92"/>
@@ -20437,7 +20430,7 @@
       <c r="H92"/>
       <c r="I92"/>
     </row>
-    <row r="93" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="93" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B93"/>
       <c r="C93"/>
       <c r="D93"/>
@@ -20447,7 +20440,7 @@
       <c r="H93"/>
       <c r="I93"/>
     </row>
-    <row r="94" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="94" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B94"/>
       <c r="C94"/>
       <c r="D94"/>
@@ -20457,7 +20450,7 @@
       <c r="H94"/>
       <c r="I94"/>
     </row>
-    <row r="95" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="95" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B95"/>
       <c r="C95"/>
       <c r="D95"/>
@@ -20467,7 +20460,7 @@
       <c r="H95"/>
       <c r="I95"/>
     </row>
-    <row r="96" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="96" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B96"/>
       <c r="C96"/>
       <c r="D96"/>
@@ -20477,7 +20470,7 @@
       <c r="H96"/>
       <c r="I96"/>
     </row>
-    <row r="97" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="97" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B97"/>
       <c r="C97"/>
       <c r="D97"/>
@@ -20487,7 +20480,7 @@
       <c r="H97"/>
       <c r="I97"/>
     </row>
-    <row r="98" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="98" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B98"/>
       <c r="C98"/>
       <c r="D98"/>
@@ -20497,7 +20490,7 @@
       <c r="H98"/>
       <c r="I98"/>
     </row>
-    <row r="99" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="99" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B99"/>
       <c r="C99"/>
       <c r="D99"/>
@@ -20507,7 +20500,7 @@
       <c r="H99"/>
       <c r="I99"/>
     </row>
-    <row r="100" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="100" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B100"/>
       <c r="C100"/>
       <c r="D100"/>
@@ -20517,7 +20510,7 @@
       <c r="H100"/>
       <c r="I100"/>
     </row>
-    <row r="101" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="101" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B101"/>
       <c r="C101"/>
       <c r="D101"/>
@@ -20527,7 +20520,7 @@
       <c r="H101"/>
       <c r="I101"/>
     </row>
-    <row r="102" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="102" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B102"/>
       <c r="C102"/>
       <c r="D102"/>
@@ -20537,7 +20530,7 @@
       <c r="H102"/>
       <c r="I102"/>
     </row>
-    <row r="103" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="103" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B103"/>
       <c r="C103"/>
       <c r="D103"/>
@@ -20547,7 +20540,7 @@
       <c r="H103"/>
       <c r="I103"/>
     </row>
-    <row r="104" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="104" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B104"/>
       <c r="C104"/>
       <c r="D104"/>
@@ -20557,7 +20550,7 @@
       <c r="H104"/>
       <c r="I104"/>
     </row>
-    <row r="105" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="105" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B105"/>
       <c r="C105"/>
       <c r="D105"/>
@@ -20567,7 +20560,7 @@
       <c r="H105"/>
       <c r="I105"/>
     </row>
-    <row r="106" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="106" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B106"/>
       <c r="C106"/>
       <c r="D106"/>
@@ -20577,7 +20570,7 @@
       <c r="H106"/>
       <c r="I106"/>
     </row>
-    <row r="107" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="107" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B107"/>
       <c r="C107"/>
       <c r="D107"/>
@@ -20587,7 +20580,7 @@
       <c r="H107"/>
       <c r="I107"/>
     </row>
-    <row r="108" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="108" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B108"/>
       <c r="C108"/>
       <c r="D108"/>
@@ -20597,7 +20590,7 @@
       <c r="H108"/>
       <c r="I108"/>
     </row>
-    <row r="109" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="109" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B109"/>
       <c r="C109"/>
       <c r="D109"/>
@@ -20607,7 +20600,7 @@
       <c r="H109"/>
       <c r="I109"/>
     </row>
-    <row r="110" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="110" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B110"/>
       <c r="C110"/>
       <c r="D110"/>
@@ -20617,7 +20610,7 @@
       <c r="H110"/>
       <c r="I110"/>
     </row>
-    <row r="111" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="111" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B111"/>
       <c r="C111"/>
       <c r="D111"/>
@@ -20627,7 +20620,7 @@
       <c r="H111"/>
       <c r="I111"/>
     </row>
-    <row r="112" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="112" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B112"/>
       <c r="C112"/>
       <c r="D112"/>
@@ -20637,7 +20630,7 @@
       <c r="H112"/>
       <c r="I112"/>
     </row>
-    <row r="113" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="113" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B113"/>
       <c r="C113"/>
       <c r="D113"/>
@@ -20647,7 +20640,7 @@
       <c r="H113"/>
       <c r="I113"/>
     </row>
-    <row r="114" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="114" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B114"/>
       <c r="C114"/>
       <c r="D114"/>
@@ -20657,7 +20650,7 @@
       <c r="H114"/>
       <c r="I114"/>
     </row>
-    <row r="115" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="115" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B115"/>
       <c r="C115"/>
       <c r="D115"/>
@@ -20667,7 +20660,7 @@
       <c r="H115"/>
       <c r="I115"/>
     </row>
-    <row r="116" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="116" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B116"/>
       <c r="C116"/>
       <c r="D116"/>
@@ -20677,7 +20670,7 @@
       <c r="H116"/>
       <c r="I116"/>
     </row>
-    <row r="117" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="117" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B117"/>
       <c r="C117"/>
       <c r="D117"/>
@@ -20687,7 +20680,7 @@
       <c r="H117"/>
       <c r="I117"/>
     </row>
-    <row r="118" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="118" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B118"/>
       <c r="C118"/>
       <c r="D118"/>
@@ -20697,7 +20690,7 @@
       <c r="H118"/>
       <c r="I118"/>
     </row>
-    <row r="119" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="119" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B119"/>
       <c r="C119"/>
       <c r="D119"/>
@@ -20707,7 +20700,7 @@
       <c r="H119"/>
       <c r="I119"/>
     </row>
-    <row r="120" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="120" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B120"/>
       <c r="C120"/>
       <c r="D120"/>
@@ -20717,7 +20710,7 @@
       <c r="H120"/>
       <c r="I120"/>
     </row>
-    <row r="121" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="121" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B121"/>
       <c r="C121"/>
       <c r="D121"/>
@@ -20727,7 +20720,7 @@
       <c r="H121"/>
       <c r="I121"/>
     </row>
-    <row r="122" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="122" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B122"/>
       <c r="C122"/>
       <c r="D122"/>
@@ -20737,7 +20730,7 @@
       <c r="H122"/>
       <c r="I122"/>
     </row>
-    <row r="123" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="123" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B123"/>
       <c r="C123"/>
       <c r="D123"/>
@@ -20747,7 +20740,7 @@
       <c r="H123"/>
       <c r="I123"/>
     </row>
-    <row r="124" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="124" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B124"/>
       <c r="C124"/>
       <c r="D124"/>
@@ -20757,7 +20750,7 @@
       <c r="H124"/>
       <c r="I124"/>
     </row>
-    <row r="125" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="125" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B125"/>
       <c r="C125"/>
       <c r="D125"/>
@@ -20767,7 +20760,7 @@
       <c r="H125"/>
       <c r="I125"/>
     </row>
-    <row r="126" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="126" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B126"/>
       <c r="C126"/>
       <c r="D126"/>
@@ -20777,7 +20770,7 @@
       <c r="H126"/>
       <c r="I126"/>
     </row>
-    <row r="127" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="127" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B127"/>
       <c r="C127"/>
       <c r="D127"/>
@@ -20787,7 +20780,7 @@
       <c r="H127"/>
       <c r="I127"/>
     </row>
-    <row r="128" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="128" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B128"/>
       <c r="C128"/>
       <c r="D128"/>
@@ -20797,7 +20790,7 @@
       <c r="H128"/>
       <c r="I128"/>
     </row>
-    <row r="129" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="129" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B129"/>
       <c r="C129"/>
       <c r="D129"/>
@@ -20807,7 +20800,7 @@
       <c r="H129"/>
       <c r="I129"/>
     </row>
-    <row r="130" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="130" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B130"/>
       <c r="C130"/>
       <c r="D130"/>
@@ -20817,7 +20810,7 @@
       <c r="H130"/>
       <c r="I130"/>
     </row>
-    <row r="131" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="131" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B131"/>
       <c r="C131"/>
       <c r="D131"/>
@@ -20827,7 +20820,7 @@
       <c r="H131"/>
       <c r="I131"/>
     </row>
-    <row r="132" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="132" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B132"/>
       <c r="C132"/>
       <c r="D132"/>
@@ -20837,7 +20830,7 @@
       <c r="H132"/>
       <c r="I132"/>
     </row>
-    <row r="133" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="133" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B133"/>
       <c r="C133"/>
       <c r="D133"/>
@@ -20847,7 +20840,7 @@
       <c r="H133"/>
       <c r="I133"/>
     </row>
-    <row r="134" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="134" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B134"/>
       <c r="C134"/>
       <c r="D134"/>
@@ -20857,7 +20850,7 @@
       <c r="H134"/>
       <c r="I134"/>
     </row>
-    <row r="135" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="135" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B135"/>
       <c r="C135"/>
       <c r="D135"/>
@@ -20867,7 +20860,7 @@
       <c r="H135"/>
       <c r="I135"/>
     </row>
-    <row r="136" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="136" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B136"/>
       <c r="C136"/>
       <c r="D136"/>
@@ -20877,7 +20870,7 @@
       <c r="H136"/>
       <c r="I136"/>
     </row>
-    <row r="137" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="137" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B137"/>
       <c r="C137"/>
       <c r="D137"/>
@@ -20887,7 +20880,7 @@
       <c r="H137"/>
       <c r="I137"/>
     </row>
-    <row r="138" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="138" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B138"/>
       <c r="C138"/>
       <c r="D138"/>
@@ -20897,7 +20890,7 @@
       <c r="H138"/>
       <c r="I138"/>
     </row>
-    <row r="139" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="139" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B139"/>
       <c r="C139"/>
       <c r="D139"/>
@@ -20907,7 +20900,7 @@
       <c r="H139"/>
       <c r="I139"/>
     </row>
-    <row r="140" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="140" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B140"/>
       <c r="C140"/>
       <c r="D140"/>
@@ -20917,7 +20910,7 @@
       <c r="H140"/>
       <c r="I140"/>
     </row>
-    <row r="141" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="141" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B141"/>
       <c r="C141"/>
       <c r="D141"/>
@@ -20927,7 +20920,7 @@
       <c r="H141"/>
       <c r="I141"/>
     </row>
-    <row r="142" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="142" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B142"/>
       <c r="C142"/>
       <c r="D142"/>
@@ -20937,7 +20930,7 @@
       <c r="H142"/>
       <c r="I142"/>
     </row>
-    <row r="143" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="143" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B143"/>
       <c r="C143"/>
       <c r="D143"/>
@@ -20947,7 +20940,7 @@
       <c r="H143"/>
       <c r="I143"/>
     </row>
-    <row r="144" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="144" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B144"/>
       <c r="C144"/>
       <c r="D144"/>
@@ -20970,15 +20963,15 @@
       <selection sqref="A1:B6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData>
-    <row r="1" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" ht="16" x14ac:dyDescent="0.4">
       <c r="A1" s="3" t="s">
         <v>23</v>
       </c>
       <c r="B1" s="3"/>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>24</v>
       </c>
@@ -20986,7 +20979,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>26</v>
       </c>
@@ -20994,7 +20987,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>27</v>
       </c>
@@ -21002,7 +20995,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>28</v>
       </c>
@@ -21010,7 +21003,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>29</v>
       </c>

</xml_diff>